<commit_message>
latest charts and excels
</commit_message>
<xml_diff>
--- a/excels/elstat/formated epipedo ekpaideusis.xlsx
+++ b/excels/elstat/formated epipedo ekpaideusis.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="39">
   <si>
     <t>Total</t>
   </si>
@@ -71,9 +71,15 @@
     <t xml:space="preserve"> Eastern Macedonia and Thrace, Greece</t>
   </si>
   <si>
+    <t>Eastern Macedonia and Thrace, Greece</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Central Macedonia, Greece</t>
   </si>
   <si>
+    <t>Central Macedonia, Greece</t>
+  </si>
+  <si>
     <t>Western Macedonia, Greece</t>
   </si>
   <si>
@@ -83,22 +89,40 @@
     <t xml:space="preserve"> Thessaly, Greece</t>
   </si>
   <si>
+    <t>Thessaly, Greece</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Central Greece (region), Greece</t>
   </si>
   <si>
+    <t>Central Greece (region), Greece</t>
+  </si>
+  <si>
     <t>Ionian Islands (region), Greece</t>
   </si>
   <si>
     <t xml:space="preserve"> Western Greece, Greece</t>
   </si>
   <si>
+    <t>Western Greece, Greece</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Peloponnese (region), Greece</t>
   </si>
   <si>
+    <t>Peloponnese (region), Greece</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Attica (region), Greece</t>
   </si>
   <si>
+    <t>Attica (region), Greece</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Northern Aegean, Greece</t>
+  </si>
+  <si>
+    <t>Northern Aegean, Greece</t>
   </si>
   <si>
     <t>Southern Aegean, Greece</t>
@@ -130,7 +154,7 @@
       <name val="Arial Narrow"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -141,12 +165,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFE7F9EF"/>
         <bgColor rgb="FFE7F9EF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -206,21 +224,41 @@
     <xf borderId="0" fillId="2" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
     <dxf>
       <font/>
       <fill>
         <patternFill patternType="none"/>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE7F9EF"/>
+          <bgColor rgb="FFE7F9EF"/>
+        </patternFill>
       </fill>
       <border/>
     </dxf>
@@ -238,16 +276,6 @@
       <font/>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor rgb="FFF3F3F3"/>
           <bgColor rgb="FFF3F3F3"/>
         </patternFill>
@@ -255,11 +283,15 @@
       <border/>
     </dxf>
   </dxfs>
-  <tableStyles count="1">
-    <tableStyle count="3" pivot="0" name="Φύλλο1-style">
-      <tableStyleElement dxfId="1" type="headerRow"/>
-      <tableStyleElement dxfId="2" type="firstRowStripe"/>
-      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+  <tableStyles count="2">
+    <tableStyle count="2" pivot="0" name="Φύλλο1-style">
+      <tableStyleElement dxfId="1" type="firstRowStripe"/>
+      <tableStyleElement dxfId="2" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="3" pivot="0" name="Φύλλο1-style 2">
+      <tableStyleElement dxfId="3" type="headerRow"/>
+      <tableStyleElement dxfId="1" type="firstRowStripe"/>
+      <tableStyleElement dxfId="4" type="secondRowStripe"/>
     </tableStyle>
   </tableStyles>
 </styleSheet>
@@ -270,7 +302,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="C1:R1" displayName="Table_1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A4:R29" displayName="Table_1" id="1">
+  <tableColumns count="18">
+    <tableColumn name="Column1" id="1"/>
+    <tableColumn name="Column2" id="2"/>
+    <tableColumn name="Column3" id="3"/>
+    <tableColumn name="Column4" id="4"/>
+    <tableColumn name="Column5" id="5"/>
+    <tableColumn name="Column6" id="6"/>
+    <tableColumn name="Column7" id="7"/>
+    <tableColumn name="Column8" id="8"/>
+    <tableColumn name="Column9" id="9"/>
+    <tableColumn name="Column10" id="10"/>
+    <tableColumn name="Column11" id="11"/>
+    <tableColumn name="Column12" id="12"/>
+    <tableColumn name="Column13" id="13"/>
+    <tableColumn name="Column14" id="14"/>
+    <tableColumn name="Column15" id="15"/>
+    <tableColumn name="Column16" id="16"/>
+    <tableColumn name="Column17" id="17"/>
+    <tableColumn name="Column18" id="18"/>
+  </tableColumns>
+  <tableStyleInfo name="Φύλλο1-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="C1:R1" displayName="Table_2" id="2">
   <tableColumns count="16">
     <tableColumn name="Column1" id="1"/>
     <tableColumn name="Column2" id="2"/>
@@ -289,7 +347,7 @@
     <tableColumn name="Column15" id="15"/>
     <tableColumn name="Column16" id="16"/>
   </tableColumns>
-  <tableStyleInfo name="Φύλλο1-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="Φύλλο1-style 2" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" headerRowCount="1"/>
@@ -410,6 +468,9 @@
       </c>
     </row>
     <row r="3">
+      <c r="A3" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="B3" s="3" t="s">
         <v>17</v>
       </c>
@@ -463,1387 +524,1411 @@
       <c r="A4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="5">
         <v>299643.0</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="5">
         <v>754.0</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="5">
         <v>1962.0</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="5">
         <v>20944.0</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="5">
         <v>10479.0</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="5">
         <v>1754.0</v>
       </c>
-      <c r="I4" s="9">
+      <c r="I4" s="5">
         <v>8876.0</v>
       </c>
-      <c r="J4" s="9">
+      <c r="J4" s="5">
         <v>45419.0</v>
       </c>
-      <c r="K4" s="9">
+      <c r="K4" s="5">
         <v>15835.0</v>
       </c>
-      <c r="L4" s="9">
+      <c r="L4" s="5">
         <v>11556.0</v>
       </c>
-      <c r="M4" s="9">
+      <c r="M4" s="5">
         <v>31386.0</v>
       </c>
-      <c r="N4" s="9">
+      <c r="N4" s="5">
         <v>87924.0</v>
       </c>
-      <c r="O4" s="9">
+      <c r="O4" s="5">
         <v>15307.0</v>
       </c>
-      <c r="P4" s="9">
+      <c r="P4" s="5">
         <v>19599.0</v>
       </c>
-      <c r="Q4" s="9">
+      <c r="Q4" s="5">
         <v>8000.0</v>
       </c>
-      <c r="R4" s="9"/>
+      <c r="R4" s="5"/>
     </row>
     <row r="5">
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>308539.0</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>317.0</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>1870.0</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <v>21977.0</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <v>10659.0</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="5">
         <v>1032.0</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="5">
         <v>11758.0</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="5">
         <v>45823.0</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="5">
         <v>7906.0</v>
       </c>
-      <c r="L5" s="6">
+      <c r="L5" s="5">
         <v>3819.0</v>
       </c>
-      <c r="M5" s="6">
+      <c r="M5" s="5">
         <v>26176.0</v>
       </c>
-      <c r="N5" s="6">
+      <c r="N5" s="5">
         <v>97097.0</v>
       </c>
-      <c r="O5" s="6">
+      <c r="O5" s="5">
         <v>24695.0</v>
       </c>
-      <c r="P5" s="6">
+      <c r="P5" s="5">
         <v>18845.0</v>
       </c>
-      <c r="Q5" s="6">
+      <c r="Q5" s="5">
         <v>17743.0</v>
       </c>
-      <c r="R5" s="6"/>
+      <c r="R5" s="5"/>
     </row>
     <row r="6">
       <c r="A6" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="5">
         <v>912693.0</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="5">
         <v>5019.0</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="5">
         <v>11549.0</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="5">
         <v>84193.0</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="5">
         <v>36248.0</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="5">
         <v>6680.0</v>
       </c>
-      <c r="I6" s="9">
+      <c r="I6" s="5">
         <v>36218.0</v>
       </c>
-      <c r="J6" s="9">
+      <c r="J6" s="5">
         <v>166400.0</v>
       </c>
-      <c r="K6" s="9">
+      <c r="K6" s="5">
         <v>48136.0</v>
       </c>
-      <c r="L6" s="9">
+      <c r="L6" s="5">
         <v>36273.0</v>
       </c>
-      <c r="M6" s="9">
+      <c r="M6" s="5">
         <v>106736.0</v>
       </c>
-      <c r="N6" s="9">
+      <c r="N6" s="5">
         <v>209866.0</v>
       </c>
-      <c r="O6" s="9">
+      <c r="O6" s="5">
         <v>32453.0</v>
       </c>
-      <c r="P6" s="9">
+      <c r="P6" s="5">
         <v>60182.0</v>
       </c>
-      <c r="Q6" s="9">
+      <c r="Q6" s="5">
         <v>10873.0</v>
       </c>
-      <c r="R6" s="9"/>
+      <c r="R6" s="5"/>
     </row>
     <row r="7">
-      <c r="B7" s="3" t="s">
+      <c r="A7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>969415.0</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>2658.0</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>11307.0</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <v>99247.0</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="5">
         <v>42932.0</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="5">
         <v>3824.0</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="5">
         <v>48768.0</v>
       </c>
-      <c r="J7" s="6">
+      <c r="J7" s="5">
         <v>186763.0</v>
       </c>
-      <c r="K7" s="6">
+      <c r="K7" s="5">
         <v>25546.0</v>
       </c>
-      <c r="L7" s="6">
+      <c r="L7" s="5">
         <v>13345.0</v>
       </c>
-      <c r="M7" s="6">
+      <c r="M7" s="5">
         <v>97611.0</v>
       </c>
-      <c r="N7" s="6">
+      <c r="N7" s="5">
         <v>241605.0</v>
       </c>
-      <c r="O7" s="6">
+      <c r="O7" s="5">
         <v>56018.0</v>
       </c>
-      <c r="P7" s="6">
+      <c r="P7" s="5">
         <v>58295.0</v>
       </c>
-      <c r="Q7" s="6">
+      <c r="Q7" s="5">
         <v>22240.0</v>
       </c>
-      <c r="R7" s="6"/>
+      <c r="R7" s="5"/>
     </row>
     <row r="8">
       <c r="A8" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="5">
         <v>141779.0</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="5">
         <v>235.0</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="5">
         <v>811.0</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="5">
         <v>9511.0</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="5">
         <v>5710.0</v>
       </c>
-      <c r="H8" s="9">
+      <c r="H8" s="5">
         <v>829.0</v>
       </c>
-      <c r="I8" s="9">
+      <c r="I8" s="5">
         <v>4628.0</v>
       </c>
-      <c r="J8" s="9">
+      <c r="J8" s="5">
         <v>20744.0</v>
       </c>
-      <c r="K8" s="9">
+      <c r="K8" s="5">
         <v>9373.0</v>
       </c>
-      <c r="L8" s="9">
+      <c r="L8" s="5">
         <v>9137.0</v>
       </c>
-      <c r="M8" s="9">
+      <c r="M8" s="5">
         <v>15551.0</v>
       </c>
-      <c r="N8" s="9">
+      <c r="N8" s="5">
         <v>39013.0</v>
       </c>
-      <c r="O8" s="9">
+      <c r="O8" s="5">
         <v>6970.0</v>
       </c>
-      <c r="P8" s="9">
+      <c r="P8" s="5">
         <v>8967.0</v>
       </c>
-      <c r="Q8" s="9">
+      <c r="Q8" s="5">
         <v>1770.0</v>
       </c>
-      <c r="R8" s="9"/>
+      <c r="R8" s="5"/>
     </row>
     <row r="9">
-      <c r="B9" s="3" t="s">
+      <c r="A9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>141910.0</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>108.0</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>777.0</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="5">
         <v>10759.0</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="5">
         <v>6476.0</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="5">
         <v>333.0</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="5">
         <v>5350.0</v>
       </c>
-      <c r="J9" s="6">
+      <c r="J9" s="5">
         <v>22202.0</v>
       </c>
-      <c r="K9" s="6">
+      <c r="K9" s="5">
         <v>4341.0</v>
       </c>
-      <c r="L9" s="6">
+      <c r="L9" s="5">
         <v>2139.0</v>
       </c>
-      <c r="M9" s="6">
+      <c r="M9" s="5">
         <v>14043.0</v>
       </c>
-      <c r="N9" s="6">
+      <c r="N9" s="5">
         <v>43176.0</v>
       </c>
-      <c r="O9" s="6">
+      <c r="O9" s="5">
         <v>11158.0</v>
       </c>
-      <c r="P9" s="6">
+      <c r="P9" s="5">
         <v>8693.0</v>
       </c>
-      <c r="Q9" s="6">
+      <c r="Q9" s="5">
         <v>4220.0</v>
       </c>
-      <c r="R9" s="6"/>
+      <c r="R9" s="5"/>
     </row>
     <row r="10">
       <c r="A10" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="5">
         <v>165775.0</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="5">
         <v>705.0</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="5">
         <v>1124.0</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="5">
         <v>14413.0</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="5">
         <v>5936.0</v>
       </c>
-      <c r="H10" s="9">
+      <c r="H10" s="5">
         <v>1099.0</v>
       </c>
-      <c r="I10" s="9">
+      <c r="I10" s="5">
         <v>4580.0</v>
       </c>
-      <c r="J10" s="9">
+      <c r="J10" s="5">
         <v>28968.0</v>
       </c>
-      <c r="K10" s="9">
+      <c r="K10" s="5">
         <v>6299.0</v>
       </c>
-      <c r="L10" s="9">
+      <c r="L10" s="5">
         <v>5002.0</v>
       </c>
-      <c r="M10" s="9">
+      <c r="M10" s="5">
         <v>19471.0</v>
       </c>
-      <c r="N10" s="9">
+      <c r="N10" s="5">
         <v>48693.0</v>
       </c>
-      <c r="O10" s="9">
+      <c r="O10" s="5">
         <v>7252.0</v>
       </c>
-      <c r="P10" s="9">
+      <c r="P10" s="5">
         <v>9545.0</v>
       </c>
-      <c r="Q10" s="9">
+      <c r="Q10" s="5">
         <v>2687.0</v>
       </c>
-      <c r="R10" s="9"/>
+      <c r="R10" s="5"/>
     </row>
     <row r="11">
-      <c r="B11" s="3" t="s">
+      <c r="A11" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <v>171081.0</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="5">
         <v>380.0</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <v>1191.0</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="5">
         <v>15370.0</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="5">
         <v>7008.0</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="5">
         <v>639.0</v>
       </c>
-      <c r="I11" s="6">
+      <c r="I11" s="5">
         <v>5989.0</v>
       </c>
-      <c r="J11" s="6">
+      <c r="J11" s="5">
         <v>29589.0</v>
       </c>
-      <c r="K11" s="6">
+      <c r="K11" s="5">
         <v>3075.0</v>
       </c>
-      <c r="L11" s="6">
+      <c r="L11" s="5">
         <v>2237.0</v>
       </c>
-      <c r="M11" s="6">
+      <c r="M11" s="5">
         <v>14646.0</v>
       </c>
-      <c r="N11" s="6">
+      <c r="N11" s="5">
         <v>48465.0</v>
       </c>
-      <c r="O11" s="6">
+      <c r="O11" s="5">
         <v>13176.0</v>
       </c>
-      <c r="P11" s="6">
+      <c r="P11" s="5">
         <v>9236.0</v>
       </c>
-      <c r="Q11" s="6">
+      <c r="Q11" s="5">
         <v>10863.0</v>
       </c>
-      <c r="R11" s="6"/>
+      <c r="R11" s="5"/>
     </row>
     <row r="12">
       <c r="A12" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="5">
         <v>362194.0</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="5">
         <v>904.0</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="5">
         <v>2457.0</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="5">
         <v>30446.0</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="5">
         <v>14902.0</v>
       </c>
-      <c r="H12" s="9">
+      <c r="H12" s="5">
         <v>2779.0</v>
       </c>
-      <c r="I12" s="9">
+      <c r="I12" s="5">
         <v>10908.0</v>
       </c>
-      <c r="J12" s="9">
+      <c r="J12" s="5">
         <v>62720.0</v>
       </c>
-      <c r="K12" s="9">
+      <c r="K12" s="5">
         <v>15725.0</v>
       </c>
-      <c r="L12" s="9">
+      <c r="L12" s="5">
         <v>11663.0</v>
       </c>
-      <c r="M12" s="9">
+      <c r="M12" s="5">
         <v>43318.0</v>
       </c>
-      <c r="N12" s="9">
+      <c r="N12" s="5">
         <v>95453.0</v>
       </c>
-      <c r="O12" s="9">
+      <c r="O12" s="5">
         <v>17273.0</v>
       </c>
-      <c r="P12" s="9">
+      <c r="P12" s="5">
         <v>22700.0</v>
       </c>
-      <c r="Q12" s="9">
+      <c r="Q12" s="5">
         <v>7347.0</v>
       </c>
-      <c r="R12" s="9"/>
+      <c r="R12" s="5"/>
     </row>
     <row r="13">
-      <c r="B13" s="3" t="s">
+      <c r="A13" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <v>370568.0</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="5">
         <v>471.0</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="5">
         <v>2432.0</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="5">
         <v>33125.0</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="5">
         <v>15476.0</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="5">
         <v>1191.0</v>
       </c>
-      <c r="I13" s="6">
+      <c r="I13" s="5">
         <v>14980.0</v>
       </c>
-      <c r="J13" s="6">
+      <c r="J13" s="5">
         <v>63096.0</v>
       </c>
-      <c r="K13" s="6">
+      <c r="K13" s="5">
         <v>6307.0</v>
       </c>
-      <c r="L13" s="6">
+      <c r="L13" s="5">
         <v>3134.0</v>
       </c>
-      <c r="M13" s="6">
+      <c r="M13" s="5">
         <v>33735.0</v>
       </c>
-      <c r="N13" s="6">
+      <c r="N13" s="5">
         <v>103106.0</v>
       </c>
-      <c r="O13" s="6">
+      <c r="O13" s="5">
         <v>26697.0</v>
       </c>
-      <c r="P13" s="6">
+      <c r="P13" s="5">
         <v>22059.0</v>
       </c>
-      <c r="Q13" s="6">
+      <c r="Q13" s="5">
         <v>22160.0</v>
       </c>
-      <c r="R13" s="6"/>
+      <c r="R13" s="5"/>
     </row>
     <row r="14">
       <c r="A14" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="5">
         <v>277475.0</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="5">
         <v>444.0</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="5">
         <v>1563.0</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="5">
         <v>18866.0</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="5">
         <v>10139.0</v>
       </c>
-      <c r="H14" s="9">
+      <c r="H14" s="5">
         <v>2897.0</v>
       </c>
-      <c r="I14" s="9">
+      <c r="I14" s="5">
         <v>8741.0</v>
       </c>
-      <c r="J14" s="9">
+      <c r="J14" s="5">
         <v>47114.0</v>
       </c>
-      <c r="K14" s="9">
+      <c r="K14" s="5">
         <v>13852.0</v>
       </c>
-      <c r="L14" s="9">
+      <c r="L14" s="5">
         <v>11527.0</v>
       </c>
-      <c r="M14" s="9">
+      <c r="M14" s="5">
         <v>36481.0</v>
       </c>
-      <c r="N14" s="9">
+      <c r="N14" s="5">
         <v>74644.0</v>
       </c>
-      <c r="O14" s="9">
+      <c r="O14" s="5">
         <v>10768.0</v>
       </c>
-      <c r="P14" s="9">
+      <c r="P14" s="5">
         <v>16546.0</v>
       </c>
-      <c r="Q14" s="9">
+      <c r="Q14" s="5">
         <v>7553.0</v>
       </c>
-      <c r="R14" s="9"/>
+      <c r="R14" s="5"/>
     </row>
     <row r="15">
-      <c r="B15" s="3" t="s">
+      <c r="A15" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="5">
         <v>269915.0</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="5">
         <v>177.0</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="5">
         <v>1238.0</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="5">
         <v>19874.0</v>
       </c>
-      <c r="G15" s="6">
+      <c r="G15" s="5">
         <v>8824.0</v>
       </c>
-      <c r="H15" s="6">
+      <c r="H15" s="5">
         <v>800.0</v>
       </c>
-      <c r="I15" s="6">
+      <c r="I15" s="5">
         <v>9945.0</v>
       </c>
-      <c r="J15" s="6">
+      <c r="J15" s="5">
         <v>50613.0</v>
       </c>
-      <c r="K15" s="6">
+      <c r="K15" s="5">
         <v>5888.0</v>
       </c>
-      <c r="L15" s="6">
+      <c r="L15" s="5">
         <v>2311.0</v>
       </c>
-      <c r="M15" s="6">
+      <c r="M15" s="5">
         <v>28655.0</v>
       </c>
-      <c r="N15" s="6">
+      <c r="N15" s="5">
         <v>78224.0</v>
       </c>
-      <c r="O15" s="6">
+      <c r="O15" s="5">
         <v>18297.0</v>
       </c>
-      <c r="P15" s="6">
+      <c r="P15" s="5">
         <v>15928.0</v>
       </c>
-      <c r="Q15" s="6">
+      <c r="Q15" s="5">
         <v>13723.0</v>
       </c>
-      <c r="R15" s="6"/>
+      <c r="R15" s="5"/>
     </row>
     <row r="16">
       <c r="A16" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="5">
         <v>102400.0</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="5">
         <v>191.0</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="5">
         <v>645.0</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16" s="5">
         <v>6959.0</v>
       </c>
-      <c r="G16" s="9">
+      <c r="G16" s="5">
         <v>3069.0</v>
       </c>
-      <c r="H16" s="9">
+      <c r="H16" s="5">
         <v>1396.0</v>
       </c>
-      <c r="I16" s="9">
+      <c r="I16" s="5">
         <v>3824.0</v>
       </c>
-      <c r="J16" s="9">
+      <c r="J16" s="5">
         <v>17459.0</v>
       </c>
-      <c r="K16" s="9">
+      <c r="K16" s="5">
         <v>3695.0</v>
       </c>
-      <c r="L16" s="9">
+      <c r="L16" s="5">
         <v>3081.0</v>
       </c>
-      <c r="M16" s="9">
+      <c r="M16" s="5">
         <v>14412.0</v>
       </c>
-      <c r="N16" s="9">
+      <c r="N16" s="5">
         <v>30338.0</v>
       </c>
-      <c r="O16" s="9">
+      <c r="O16" s="5">
         <v>3182.0</v>
       </c>
-      <c r="P16" s="9">
+      <c r="P16" s="5">
         <v>6184.0</v>
       </c>
-      <c r="Q16" s="9">
+      <c r="Q16" s="5">
         <v>1387.0</v>
       </c>
-      <c r="R16" s="9"/>
+      <c r="R16" s="5"/>
     </row>
     <row r="17">
-      <c r="B17" s="3" t="s">
+      <c r="A17" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="5">
         <v>105455.0</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="5">
         <v>104.0</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="5">
         <v>682.0</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="5">
         <v>8312.0</v>
       </c>
-      <c r="G17" s="6">
+      <c r="G17" s="5">
         <v>3304.0</v>
       </c>
-      <c r="H17" s="6">
+      <c r="H17" s="5">
         <v>546.0</v>
       </c>
-      <c r="I17" s="6">
+      <c r="I17" s="5">
         <v>5116.0</v>
       </c>
-      <c r="J17" s="6">
+      <c r="J17" s="5">
         <v>20127.0</v>
       </c>
-      <c r="K17" s="6">
+      <c r="K17" s="5">
         <v>1749.0</v>
       </c>
-      <c r="L17" s="6">
+      <c r="L17" s="5">
         <v>1210.0</v>
       </c>
-      <c r="M17" s="6">
+      <c r="M17" s="5">
         <v>11575.0</v>
       </c>
-      <c r="N17" s="6">
+      <c r="N17" s="5">
         <v>29345.0</v>
       </c>
-      <c r="O17" s="6">
+      <c r="O17" s="5">
         <v>5854.0</v>
       </c>
-      <c r="P17" s="6">
+      <c r="P17" s="5">
         <v>6057.0</v>
       </c>
-      <c r="Q17" s="6">
+      <c r="Q17" s="5">
         <v>5356.0</v>
       </c>
-      <c r="R17" s="6"/>
+      <c r="R17" s="5"/>
     </row>
     <row r="18">
       <c r="A18" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="5">
         <v>339310.0</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18" s="5">
         <v>1196.0</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18" s="5">
         <v>2110.0</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="5">
         <v>23402.0</v>
       </c>
-      <c r="G18" s="9">
+      <c r="G18" s="5">
         <v>10910.0</v>
       </c>
-      <c r="H18" s="9">
+      <c r="H18" s="5">
         <v>2603.0</v>
       </c>
-      <c r="I18" s="9">
+      <c r="I18" s="5">
         <v>7910.0</v>
       </c>
-      <c r="J18" s="9">
+      <c r="J18" s="5">
         <v>65688.0</v>
       </c>
-      <c r="K18" s="9">
+      <c r="K18" s="5">
         <v>13363.0</v>
       </c>
-      <c r="L18" s="9">
+      <c r="L18" s="5">
         <v>9362.0</v>
       </c>
-      <c r="M18" s="9">
+      <c r="M18" s="5">
         <v>43625.0</v>
       </c>
-      <c r="N18" s="9">
+      <c r="N18" s="5">
         <v>94683.0</v>
       </c>
-      <c r="O18" s="9">
+      <c r="O18" s="5">
         <v>12713.0</v>
       </c>
-      <c r="P18" s="9">
+      <c r="P18" s="5">
         <v>21754.0</v>
       </c>
-      <c r="Q18" s="9">
+      <c r="Q18" s="5">
         <v>8543.0</v>
       </c>
-      <c r="R18" s="9"/>
+      <c r="R18" s="5"/>
     </row>
     <row r="19">
-      <c r="B19" s="3" t="s">
+      <c r="A19" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="5">
         <v>340486.0</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="5">
         <v>532.0</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="5">
         <v>2036.0</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19" s="5">
         <v>25825.0</v>
       </c>
-      <c r="G19" s="6">
+      <c r="G19" s="5">
         <v>12884.0</v>
       </c>
-      <c r="H19" s="6">
+      <c r="H19" s="5">
         <v>1021.0</v>
       </c>
-      <c r="I19" s="6">
+      <c r="I19" s="5">
         <v>10237.0</v>
       </c>
-      <c r="J19" s="6">
+      <c r="J19" s="5">
         <v>69638.0</v>
       </c>
-      <c r="K19" s="6">
+      <c r="K19" s="5">
         <v>6746.0</v>
       </c>
-      <c r="L19" s="6">
+      <c r="L19" s="5">
         <v>2979.0</v>
       </c>
-      <c r="M19" s="6">
+      <c r="M19" s="5">
         <v>34026.0</v>
       </c>
-      <c r="N19" s="6">
+      <c r="N19" s="5">
         <v>93168.0</v>
       </c>
-      <c r="O19" s="6">
+      <c r="O19" s="5">
         <v>20728.0</v>
       </c>
-      <c r="P19" s="6">
+      <c r="P19" s="5">
         <v>21005.0</v>
       </c>
-      <c r="Q19" s="6">
+      <c r="Q19" s="5">
         <v>19455.0</v>
       </c>
-      <c r="R19" s="6"/>
+      <c r="R19" s="5"/>
     </row>
     <row r="20">
       <c r="A20" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="5">
         <v>291777.0</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="5">
         <v>472.0</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="5">
         <v>1717.0</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20" s="5">
         <v>20202.0</v>
       </c>
-      <c r="G20" s="9">
+      <c r="G20" s="5">
         <v>9352.0</v>
       </c>
-      <c r="H20" s="9">
+      <c r="H20" s="5">
         <v>2947.0</v>
       </c>
-      <c r="I20" s="9">
+      <c r="I20" s="5">
         <v>8579.0</v>
       </c>
-      <c r="J20" s="9">
+      <c r="J20" s="5">
         <v>53065.0</v>
       </c>
-      <c r="K20" s="9">
+      <c r="K20" s="5">
         <v>11845.0</v>
       </c>
-      <c r="L20" s="9">
+      <c r="L20" s="5">
         <v>9089.0</v>
       </c>
-      <c r="M20" s="9">
+      <c r="M20" s="5">
         <v>42789.0</v>
       </c>
-      <c r="N20" s="9">
+      <c r="N20" s="5">
         <v>81795.0</v>
       </c>
-      <c r="O20" s="9">
+      <c r="O20" s="5">
         <v>10854.0</v>
       </c>
-      <c r="P20" s="9">
+      <c r="P20" s="5">
         <v>17221.0</v>
       </c>
-      <c r="Q20" s="9">
+      <c r="Q20" s="5">
         <v>4575.0</v>
       </c>
-      <c r="R20" s="9"/>
+      <c r="R20" s="5"/>
     </row>
     <row r="21">
-      <c r="B21" s="3" t="s">
+      <c r="A21" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="5">
         <v>286126.0</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="5">
         <v>241.0</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="5">
         <v>1401.0</v>
       </c>
-      <c r="F21" s="6">
+      <c r="F21" s="5">
         <v>21570.0</v>
       </c>
-      <c r="G21" s="6">
+      <c r="G21" s="5">
         <v>9168.0</v>
       </c>
-      <c r="H21" s="6">
+      <c r="H21" s="5">
         <v>1105.0</v>
       </c>
-      <c r="I21" s="6">
+      <c r="I21" s="5">
         <v>10238.0</v>
       </c>
-      <c r="J21" s="6">
+      <c r="J21" s="5">
         <v>55932.0</v>
       </c>
-      <c r="K21" s="6">
+      <c r="K21" s="5">
         <v>5508.0</v>
       </c>
-      <c r="L21" s="6">
+      <c r="L21" s="5">
         <v>2570.0</v>
       </c>
-      <c r="M21" s="6">
+      <c r="M21" s="5">
         <v>33471.0</v>
       </c>
-      <c r="N21" s="6">
+      <c r="N21" s="5">
         <v>82231.0</v>
       </c>
-      <c r="O21" s="6">
+      <c r="O21" s="5">
         <v>19450.0</v>
       </c>
-      <c r="P21" s="6">
+      <c r="P21" s="5">
         <v>16661.0</v>
       </c>
-      <c r="Q21" s="6">
+      <c r="Q21" s="5">
         <v>10171.0</v>
       </c>
-      <c r="R21" s="6"/>
+      <c r="R21" s="5"/>
     </row>
     <row r="22">
       <c r="A22" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="9">
+      <c r="C22" s="5">
         <v>1845663.0</v>
       </c>
-      <c r="D22" s="9">
+      <c r="D22" s="5">
         <v>15327.0</v>
       </c>
-      <c r="E22" s="9">
+      <c r="E22" s="5">
         <v>52555.0</v>
       </c>
-      <c r="F22" s="9">
+      <c r="F22" s="5">
         <v>239163.0</v>
       </c>
-      <c r="G22" s="9">
+      <c r="G22" s="5">
         <v>90804.0</v>
       </c>
-      <c r="H22" s="9">
+      <c r="H22" s="5">
         <v>32058.0</v>
       </c>
-      <c r="I22" s="9">
+      <c r="I22" s="5">
         <v>102892.0</v>
       </c>
-      <c r="J22" s="9">
+      <c r="J22" s="5">
         <v>414685.0</v>
       </c>
-      <c r="K22" s="9">
+      <c r="K22" s="5">
         <v>71242.0</v>
       </c>
-      <c r="L22" s="9">
+      <c r="L22" s="5">
         <v>64200.0</v>
       </c>
-      <c r="M22" s="9">
+      <c r="M22" s="5">
         <v>200725.0</v>
       </c>
-      <c r="N22" s="9">
+      <c r="N22" s="5">
         <v>283723.0</v>
       </c>
-      <c r="O22" s="9">
+      <c r="O22" s="5">
         <v>30034.0</v>
       </c>
-      <c r="P22" s="9">
+      <c r="P22" s="5">
         <v>110025.0</v>
       </c>
-      <c r="Q22" s="9">
+      <c r="Q22" s="5">
         <v>17715.0</v>
       </c>
-      <c r="R22" s="9"/>
+      <c r="R22" s="5"/>
     </row>
     <row r="23">
-      <c r="B23" s="3" t="s">
+      <c r="A23" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="5">
         <v>1982771.0</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="5">
         <v>8402.0</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="5">
         <v>46493.0</v>
       </c>
-      <c r="F23" s="6">
+      <c r="F23" s="5">
         <v>264790.0</v>
       </c>
-      <c r="G23" s="6">
+      <c r="G23" s="5">
         <v>86718.0</v>
       </c>
-      <c r="H23" s="6">
+      <c r="H23" s="5">
         <v>13343.0</v>
       </c>
-      <c r="I23" s="6">
+      <c r="I23" s="5">
         <v>135237.0</v>
       </c>
-      <c r="J23" s="6">
+      <c r="J23" s="5">
         <v>509005.0</v>
       </c>
-      <c r="K23" s="6">
+      <c r="K23" s="5">
         <v>33556.0</v>
       </c>
-      <c r="L23" s="6">
+      <c r="L23" s="5">
         <v>23511.0</v>
       </c>
-      <c r="M23" s="6">
+      <c r="M23" s="5">
         <v>188901.0</v>
       </c>
-      <c r="N23" s="6">
+      <c r="N23" s="5">
         <v>362718.0</v>
       </c>
-      <c r="O23" s="6">
+      <c r="O23" s="5">
         <v>61119.0</v>
       </c>
-      <c r="P23" s="6">
+      <c r="P23" s="5">
         <v>106332.0</v>
       </c>
-      <c r="Q23" s="6">
+      <c r="Q23" s="5">
         <v>27398.0</v>
       </c>
-      <c r="R23" s="6"/>
+      <c r="R23" s="5"/>
     </row>
     <row r="24">
       <c r="A24" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C24" s="5">
         <v>99984.0</v>
       </c>
-      <c r="D24" s="9">
+      <c r="D24" s="5">
         <v>244.0</v>
       </c>
-      <c r="E24" s="9">
+      <c r="E24" s="5">
         <v>855.0</v>
       </c>
-      <c r="F24" s="9">
+      <c r="F24" s="5">
         <v>7483.0</v>
       </c>
-      <c r="G24" s="9">
+      <c r="G24" s="5">
         <v>4166.0</v>
       </c>
-      <c r="H24" s="9">
+      <c r="H24" s="5">
         <v>2158.0</v>
       </c>
-      <c r="I24" s="9">
+      <c r="I24" s="5">
         <v>3650.0</v>
       </c>
-      <c r="J24" s="9">
+      <c r="J24" s="5">
         <v>17693.0</v>
       </c>
-      <c r="K24" s="9">
+      <c r="K24" s="5">
         <v>5118.0</v>
       </c>
-      <c r="L24" s="9">
+      <c r="L24" s="5">
         <v>3943.0</v>
       </c>
-      <c r="M24" s="9">
+      <c r="M24" s="5">
         <v>11738.0</v>
       </c>
-      <c r="N24" s="9">
+      <c r="N24" s="5">
         <v>26401.0</v>
       </c>
-      <c r="O24" s="9">
+      <c r="O24" s="5">
         <v>3310.0</v>
       </c>
-      <c r="P24" s="9">
+      <c r="P24" s="5">
         <v>5816.0</v>
       </c>
-      <c r="Q24" s="9">
+      <c r="Q24" s="5">
         <v>1298.0</v>
       </c>
-      <c r="R24" s="9"/>
+      <c r="R24" s="5"/>
     </row>
     <row r="25">
-      <c r="B25" s="3" t="s">
+      <c r="A25" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="5">
         <v>99247.0</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="5">
         <v>110.0</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="5">
         <v>837.0</v>
       </c>
-      <c r="F25" s="6">
+      <c r="F25" s="5">
         <v>7785.0</v>
       </c>
-      <c r="G25" s="6">
+      <c r="G25" s="5">
         <v>3302.0</v>
       </c>
-      <c r="H25" s="6">
+      <c r="H25" s="5">
         <v>361.0</v>
       </c>
-      <c r="I25" s="6">
+      <c r="I25" s="5">
         <v>4209.0</v>
       </c>
-      <c r="J25" s="6">
+      <c r="J25" s="5">
         <v>18087.0</v>
       </c>
-      <c r="K25" s="6">
+      <c r="K25" s="5">
         <v>2287.0</v>
       </c>
-      <c r="L25" s="6">
+      <c r="L25" s="5">
         <v>1138.0</v>
       </c>
-      <c r="M25" s="6">
+      <c r="M25" s="5">
         <v>10280.0</v>
       </c>
-      <c r="N25" s="6">
+      <c r="N25" s="5">
         <v>31353.0</v>
       </c>
-      <c r="O25" s="6">
+      <c r="O25" s="5">
         <v>5642.0</v>
       </c>
-      <c r="P25" s="6">
+      <c r="P25" s="5">
         <v>5996.0</v>
       </c>
-      <c r="Q25" s="6">
+      <c r="Q25" s="5">
         <v>1932.0</v>
       </c>
-      <c r="R25" s="6"/>
+      <c r="R25" s="5"/>
     </row>
     <row r="26">
       <c r="A26" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="9">
+      <c r="C26" s="5">
         <v>155865.0</v>
       </c>
-      <c r="D26" s="9">
+      <c r="D26" s="5">
         <v>236.0</v>
       </c>
-      <c r="E26" s="9">
+      <c r="E26" s="5">
         <v>1214.0</v>
       </c>
-      <c r="F26" s="9">
+      <c r="F26" s="5">
         <v>10147.0</v>
       </c>
-      <c r="G26" s="9">
+      <c r="G26" s="5">
         <v>5266.0</v>
       </c>
-      <c r="H26" s="9">
+      <c r="H26" s="5">
         <v>2493.0</v>
       </c>
-      <c r="I26" s="9">
+      <c r="I26" s="5">
         <v>7018.0</v>
       </c>
-      <c r="J26" s="9">
+      <c r="J26" s="5">
         <v>25364.0</v>
       </c>
-      <c r="K26" s="9">
+      <c r="K26" s="5">
         <v>8145.0</v>
       </c>
-      <c r="L26" s="9">
+      <c r="L26" s="5">
         <v>5960.0</v>
       </c>
-      <c r="M26" s="9">
+      <c r="M26" s="5">
         <v>21410.0</v>
       </c>
-      <c r="N26" s="9">
+      <c r="N26" s="5">
         <v>40115.0</v>
       </c>
-      <c r="O26" s="9">
+      <c r="O26" s="5">
         <v>4590.0</v>
       </c>
-      <c r="P26" s="9">
+      <c r="P26" s="5">
         <v>10590.0</v>
       </c>
-      <c r="Q26" s="9">
+      <c r="Q26" s="5">
         <v>2349.0</v>
       </c>
-      <c r="R26" s="9"/>
+      <c r="R26" s="5"/>
     </row>
     <row r="27">
-      <c r="B27" s="3" t="s">
+      <c r="A27" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C27" s="5">
         <v>153150.0</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27" s="5">
         <v>137.0</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E27" s="5">
         <v>1084.0</v>
       </c>
-      <c r="F27" s="6">
+      <c r="F27" s="5">
         <v>11454.0</v>
       </c>
-      <c r="G27" s="6">
+      <c r="G27" s="5">
         <v>4433.0</v>
       </c>
-      <c r="H27" s="6">
+      <c r="H27" s="5">
         <v>1003.0</v>
       </c>
-      <c r="I27" s="6">
+      <c r="I27" s="5">
         <v>7768.0</v>
       </c>
-      <c r="J27" s="6">
+      <c r="J27" s="5">
         <v>29454.0</v>
       </c>
-      <c r="K27" s="6">
+      <c r="K27" s="5">
         <v>4555.0</v>
       </c>
-      <c r="L27" s="6">
+      <c r="L27" s="5">
         <v>2021.0</v>
       </c>
-      <c r="M27" s="6">
+      <c r="M27" s="5">
         <v>18768.0</v>
       </c>
-      <c r="N27" s="6">
+      <c r="N27" s="5">
         <v>41105.0</v>
       </c>
-      <c r="O27" s="6">
+      <c r="O27" s="5">
         <v>7019.0</v>
       </c>
-      <c r="P27" s="6">
+      <c r="P27" s="5">
         <v>10183.0</v>
       </c>
-      <c r="Q27" s="6">
+      <c r="Q27" s="5">
         <v>3561.0</v>
       </c>
-      <c r="R27" s="6"/>
+      <c r="R27" s="5"/>
     </row>
     <row r="28">
       <c r="A28" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="9">
+      <c r="C28" s="5">
         <v>308665.0</v>
       </c>
-      <c r="D28" s="9">
+      <c r="D28" s="5">
         <v>1249.0</v>
       </c>
-      <c r="E28" s="9">
+      <c r="E28" s="5">
         <v>2767.0</v>
       </c>
-      <c r="F28" s="9">
+      <c r="F28" s="5">
         <v>23139.0</v>
       </c>
-      <c r="G28" s="9">
+      <c r="G28" s="5">
         <v>12696.0</v>
       </c>
-      <c r="H28" s="9">
+      <c r="H28" s="5">
         <v>3823.0</v>
       </c>
-      <c r="I28" s="9">
+      <c r="I28" s="5">
         <v>10497.0</v>
       </c>
-      <c r="J28" s="9">
+      <c r="J28" s="5">
         <v>55633.0</v>
       </c>
-      <c r="K28" s="9">
+      <c r="K28" s="5">
         <v>11974.0</v>
       </c>
-      <c r="L28" s="9">
+      <c r="L28" s="5">
         <v>8654.0</v>
       </c>
-      <c r="M28" s="9">
+      <c r="M28" s="5">
         <v>40561.0</v>
       </c>
-      <c r="N28" s="9">
+      <c r="N28" s="5">
         <v>80236.0</v>
       </c>
-      <c r="O28" s="9">
+      <c r="O28" s="5">
         <v>8487.0</v>
       </c>
-      <c r="P28" s="9">
+      <c r="P28" s="5">
         <v>21920.0</v>
       </c>
-      <c r="Q28" s="9">
+      <c r="Q28" s="5">
         <v>3952.0</v>
       </c>
-      <c r="R28" s="9"/>
+      <c r="R28" s="5"/>
     </row>
     <row r="29">
-      <c r="B29" s="3" t="s">
+      <c r="A29" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C29" s="5">
         <v>314400.0</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="5">
         <v>699.0</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E29" s="5">
         <v>2855.0</v>
       </c>
-      <c r="F29" s="6">
+      <c r="F29" s="5">
         <v>27977.0</v>
       </c>
-      <c r="G29" s="6">
+      <c r="G29" s="5">
         <v>14049.0</v>
       </c>
-      <c r="H29" s="6">
+      <c r="H29" s="5">
         <v>1686.0</v>
       </c>
-      <c r="I29" s="6">
+      <c r="I29" s="5">
         <v>14163.0</v>
       </c>
-      <c r="J29" s="6">
+      <c r="J29" s="5">
         <v>62199.0</v>
       </c>
-      <c r="K29" s="6">
+      <c r="K29" s="5">
         <v>6850.0</v>
       </c>
-      <c r="L29" s="6">
+      <c r="L29" s="5">
         <v>4038.0</v>
       </c>
-      <c r="M29" s="6">
+      <c r="M29" s="5">
         <v>34501.0</v>
       </c>
-      <c r="N29" s="6">
+      <c r="N29" s="5">
         <v>79868.0</v>
       </c>
-      <c r="O29" s="6">
+      <c r="O29" s="5">
         <v>15036.0</v>
       </c>
-      <c r="P29" s="6">
+      <c r="P29" s="5">
         <v>20750.0</v>
       </c>
-      <c r="Q29" s="6">
+      <c r="Q29" s="5">
         <v>7492.0</v>
       </c>
-      <c r="R29" s="6"/>
+      <c r="R29" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A15"/>
-  </mergeCells>
   <drawing r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>